<commit_message>
add 4 commands: add, mul, div, root
</commit_message>
<xml_diff>
--- a/root/administrator/logs_file.xlsx
+++ b/root/administrator/logs_file.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,8 +440,8 @@
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="30" customWidth="1" min="3" max="3"/>
     <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-    <col width="40" customWidth="1" min="6" max="6"/>
+    <col width="50" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -479,17 +479,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2021/04/29</t>
+          <t>2021/04/30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>05:57:19</t>
+          <t>14:59:07</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>sdgsdgsdg</t>
+          <t>mjavadtatari</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -499,56 +499,56 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>pass: sdgsdg</t>
+          <t>pass: mjavadtatari</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>Failed Attempts= 1</t>
+          <t>Success</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2021/04/29</t>
+          <t>2021/04/30</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>05:59:13</t>
+          <t>14:59:17</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>fsdfs</t>
+          <t>mjavadtatari</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>login</t>
+          <t>MUL many</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>pass: sdfsd</t>
-        </is>
-      </c>
-      <c r="F3" s="3" t="inlineStr">
-        <is>
-          <t>Failed Attempts= 1</t>
+          <t>nums: 4 x 5 x 1 x 2 x 3 x 4 x 56</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Resualt= 26880.0</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2021/04/29</t>
+          <t>2021/04/30</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>06:50:49</t>
+          <t>14:59:49</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -575,44 +575,44 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2021/04/29</t>
+          <t>2021/04/30</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>06:50:58</t>
+          <t>15:00:58</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>mjavadtatari</t>
+          <t>mjavadtatario</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>set email</t>
+          <t>login</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>email :mjavadtatari98@gmail.com</t>
-        </is>
-      </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>Submited Successfully</t>
+          <t>pass: mjavadtatario</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>Failed Attempts= 1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2021/04/29</t>
+          <t>2021/04/30</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>06:51:39</t>
+          <t>15:01:00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -639,12 +639,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2021/04/29</t>
+          <t>2021/04/30</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>06:54:13</t>
+          <t>15:01:10</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -654,29 +654,29 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>login</t>
+          <t>ROOT</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>pass: mjavadtatari</t>
-        </is>
-      </c>
-      <c r="F7" s="2" t="inlineStr">
-        <is>
-          <t>Success</t>
+          <t>nums: 27.03.0</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Resualt= 3.0</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2021/04/29</t>
+          <t>2021/04/30</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>06:54:31</t>
+          <t>15:01:45</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -703,12 +703,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2021/04/29</t>
+          <t>2021/04/30</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>06:55:23</t>
+          <t>15:01:50</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -718,29 +718,29 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>login</t>
+          <t>ROOT</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>pass: mjavadtatari</t>
-        </is>
-      </c>
-      <c r="F9" s="2" t="inlineStr">
-        <is>
-          <t>Success</t>
+          <t>nums: 27.03.0</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Resualt= 3.0</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2021/04/29</t>
+          <t>2021/04/30</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>06:55:37</t>
+          <t>15:01:53</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -750,12 +750,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>login</t>
+          <t>logout</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>pass: mjavadtatari</t>
+          <t>q</t>
         </is>
       </c>
       <c r="F10" s="2" t="inlineStr">
@@ -767,12 +767,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2021/04/29</t>
+          <t>2021/04/30</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>06:56:08</t>
+          <t>15:03:25</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -799,12 +799,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2021/04/29</t>
+          <t>2021/04/30</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>06:57:08</t>
+          <t>15:03:33</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -814,15 +814,1280 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
+          <t>ROOT</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nums: 27.0 , 3.0</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Resualt= 3.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>15:03:36</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>logout</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>15:05:30</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>mjavadtatati</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>login</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatati</t>
+        </is>
+      </c>
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>Failed Attempts= 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>15:05:33</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>pass: mjavadtatari</t>
         </is>
       </c>
-      <c r="F12" s="2" t="inlineStr">
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>15:07:12</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>15:07:20</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>ROOT</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>nums:  , qs</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Canceled</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>15:08:55</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>15:09:00</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>ROOT</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>nums: sd</t>
+        </is>
+      </c>
+      <c r="F19" s="3" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>15:09:06</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>ROOT</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>nums: 27s</t>
+        </is>
+      </c>
+      <c r="F20" s="3" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>15:09:09</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>ROOT</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>nums: 27.0 , 3.0</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Resualt= 3.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>15:09:12</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>logout</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>15:10:26</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>15:10:28</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>ROOT</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>nums: 27.0 , 3.0</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Resualt= 3.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>15:10:33</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>ROOT</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>nums: 27.0 , 3.0</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Resualt= 3.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>15:11:19</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>15:11:32</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>ROOT</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>nums: 27.0 , 3.0</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Resualt= 3.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>15:11:38</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>ROOT</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>nums: 27.0 , 3.0</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Resualt= 3.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>15:11:41</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>ROOT</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>nums: 27 , s</t>
+        </is>
+      </c>
+      <c r="F29" s="3" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>15:11:44</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>ROOT</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>nums: s , s</t>
+        </is>
+      </c>
+      <c r="F30" s="3" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>15:11:50</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>ROOT</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>nums: q , None</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Canceled</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>15:11:51</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>logout</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>15:15:48</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>15:16:40</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>15:16:45</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>SUB</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>nums: 5 - 2</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Resualt= -7.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>15:18:38</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>15:18:47</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>ADD (many)</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>nums: 5 + -2</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Resualt= 3.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>15:18:53</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>logout</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>logout</t>
+        </is>
+      </c>
+      <c r="F38" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>15:22:17</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>15:22:33</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>DIV</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>nums: 15 / 3</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Resualt= 0.022222222222222223</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>15:23:03</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>DIV (many)</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>nums: 15 / 3</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Resualt= 0.022222222222222223</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>15:26:32</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>15:26:35</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>sd</t>
+        </is>
+      </c>
+      <c r="F43" s="3" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>15:26:36</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>sf</t>
+        </is>
+      </c>
+      <c r="F44" s="3" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>15:26:36</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>v</t>
+        </is>
+      </c>
+      <c r="F45" s="3" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>15:26:38</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>logout</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>q</t>
+        </is>
+      </c>
+      <c r="F46" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>15:30:42</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F47" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>15:33:43</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F48" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>15:33:50</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>DIV (many)</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>nums: 15 / 3</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Resualt= 5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>15:33:55</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>DIV</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>nums: 15 / 3</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Resualt= 5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>15:34:02</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>DIV</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>nums: 5 / 2</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Resualt= 2.5</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2021/04/30</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>15:34:09</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>logout</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>stop</t>
+        </is>
+      </c>
+      <c r="F52" s="2" t="inlineStr">
         <is>
           <t>Success</t>
         </is>

</xml_diff>

<commit_message>
added two (DED and SUBD) commands!
</commit_message>
<xml_diff>
--- a/root/administrator/logs_file.xlsx
+++ b/root/administrator/logs_file.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F322"/>
+  <dimension ref="A1:F426"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10698,6 +10698,3305 @@
         </is>
       </c>
     </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>19:32:00</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F323" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>19:32:06</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>HOME</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F324" s="2" t="inlineStr">
+        <is>
+          <t>Directory Changed Successfully</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>19:32:18</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>MKD</t>
+        </is>
+      </c>
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\sd.sd\</t>
+        </is>
+      </c>
+      <c r="F325" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Created!</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>19:32:42</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F326" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>19:32:44</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\</t>
+        </is>
+      </c>
+      <c r="F327" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>19:32:47</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>Not Valid</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>chd..</t>
+        </is>
+      </c>
+      <c r="F328" s="3" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>19:32:55</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\..</t>
+        </is>
+      </c>
+      <c r="F329" s="3" t="inlineStr">
+        <is>
+          <t>Failed. Try Reaching the Root!</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>19:36:50</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F330" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>19:37:02</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\sd.sd</t>
+        </is>
+      </c>
+      <c r="F331" s="3" t="inlineStr">
+        <is>
+          <t>Failed. the Directory does not exist</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>19:37:11</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\mjavadtatari\home\sd.sd</t>
+        </is>
+      </c>
+      <c r="F332" s="3" t="inlineStr">
+        <is>
+          <t>Failed. the Directory does not exist</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>19:37:21</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F333" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>19:37:27</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\sd.sd</t>
+        </is>
+      </c>
+      <c r="F334" s="3" t="inlineStr">
+        <is>
+          <t>Failed. the Directory does not exist</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>19:37:41</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\sd.sd</t>
+        </is>
+      </c>
+      <c r="F335" s="3" t="inlineStr">
+        <is>
+          <t>Failed. the Directory does not exist</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>19:37:51</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\'sd.sd'</t>
+        </is>
+      </c>
+      <c r="F336" s="3" t="inlineStr">
+        <is>
+          <t>Failed. the Directory does not exist</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>19:38:22</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F337" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>19:38:26</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>Not Valid</t>
+        </is>
+      </c>
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>ded</t>
+        </is>
+      </c>
+      <c r="F338" s="3" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>19:39:41</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E339" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F339" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>19:39:44</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>Not Valid</t>
+        </is>
+      </c>
+      <c r="E340" t="inlineStr">
+        <is>
+          <t>ded</t>
+        </is>
+      </c>
+      <c r="F340" s="3" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>19:39:54</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>Not Valid</t>
+        </is>
+      </c>
+      <c r="E341" t="inlineStr">
+        <is>
+          <t>ded</t>
+        </is>
+      </c>
+      <c r="F341" s="3" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>19:41:56</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E342" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F342" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>19:42:47</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E343" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F343" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>19:43:48</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E344" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F344" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>19:45:07</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E345" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F345" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>19:46:58</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F346" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>19:47:05</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E347" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F347" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>19:47:11</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E348" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\hello\</t>
+        </is>
+      </c>
+      <c r="F348" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>19:47:23</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D349" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E349" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\hello\byr</t>
+        </is>
+      </c>
+      <c r="F349" s="3" t="inlineStr">
+        <is>
+          <t>Failed. the Directory does not exist</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>19:47:25</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E350" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\hello\bye\</t>
+        </is>
+      </c>
+      <c r="F350" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>19:47:38</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\hello\</t>
+        </is>
+      </c>
+      <c r="F351" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>19:52:04</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F352" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>19:52:08</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>DED</t>
+        </is>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F353" s="3" t="inlineStr">
+        <is>
+          <t>Fail. Directory is Not Empty!</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>19:52:17</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>DED</t>
+        </is>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\asda\</t>
+        </is>
+      </c>
+      <c r="F354" s="3" t="inlineStr">
+        <is>
+          <t>Fail. Directory Does Not Exists!</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>19:54:46</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>mjavadtatariu</t>
+        </is>
+      </c>
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E355" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatariu</t>
+        </is>
+      </c>
+      <c r="F355" s="3" t="inlineStr">
+        <is>
+          <t>Failed Attempts= 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>19:54:50</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E356" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F356" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>19:54:57</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E357" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F357" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>19:55:07</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>DED</t>
+        </is>
+      </c>
+      <c r="E358" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\rf\</t>
+        </is>
+      </c>
+      <c r="F358" s="3" t="inlineStr">
+        <is>
+          <t>Fail. Directory Does Not Exists!</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>19:57:27</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E359" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F359" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>19:57:30</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F360" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>19:58:00</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E361" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F361" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>19:58:03</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E362" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F362" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>19:58:10</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>DED</t>
+        </is>
+      </c>
+      <c r="E363" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\hello\</t>
+        </is>
+      </c>
+      <c r="F363" s="3" t="inlineStr">
+        <is>
+          <t>Fail. Directory is Not Empty!</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>19:58:26</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E364" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\hello</t>
+        </is>
+      </c>
+      <c r="F364" s="3" t="inlineStr">
+        <is>
+          <t>Failed. the Directory does not exist</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>20:00:10</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E365" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F365" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>20:00:13</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>HOME</t>
+        </is>
+      </c>
+      <c r="E366" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F366" s="2" t="inlineStr">
+        <is>
+          <t>Directory Changed Successfully</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>20:00:18</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>MKD</t>
+        </is>
+      </c>
+      <c r="E367" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\hello\</t>
+        </is>
+      </c>
+      <c r="F367" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Created!</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>20:00:22</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>MKD</t>
+        </is>
+      </c>
+      <c r="E368" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\hello\bye\</t>
+        </is>
+      </c>
+      <c r="F368" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Created!</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>20:00:27</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D369" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E369" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\hello\</t>
+        </is>
+      </c>
+      <c r="F369" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>20:00:28</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E370" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F370" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>20:00:33</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D371" t="inlineStr">
+        <is>
+          <t>DED</t>
+        </is>
+      </c>
+      <c r="E371" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\hello\</t>
+        </is>
+      </c>
+      <c r="F371" s="3" t="inlineStr">
+        <is>
+          <t>Fail. Directory is Not Empty!</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>20:00:41</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D372" t="inlineStr">
+        <is>
+          <t>DED RF</t>
+        </is>
+      </c>
+      <c r="E372" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\hello\</t>
+        </is>
+      </c>
+      <c r="F372" s="2" t="inlineStr">
+        <is>
+          <t>Success. the Directory and its Content Deleted!</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>20:08:05</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D373" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E373" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F373" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>20:08:09</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D374" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E374" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F374" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>20:08:14</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>MKD</t>
+        </is>
+      </c>
+      <c r="E375" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\hello\</t>
+        </is>
+      </c>
+      <c r="F375" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Created!</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>20:08:18</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>MKD</t>
+        </is>
+      </c>
+      <c r="E376" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\hello\bye\</t>
+        </is>
+      </c>
+      <c r="F376" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Created!</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>20:08:23</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\hello\</t>
+        </is>
+      </c>
+      <c r="F377" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>20:08:24</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F378" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>20:08:42</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>DED</t>
+        </is>
+      </c>
+      <c r="E379" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\hello\</t>
+        </is>
+      </c>
+      <c r="F379" s="3" t="inlineStr">
+        <is>
+          <t>Failed. Directory is Not Empty!</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>20:08:48</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>DED RF</t>
+        </is>
+      </c>
+      <c r="E380" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\hello\</t>
+        </is>
+      </c>
+      <c r="F380" s="2" t="inlineStr">
+        <is>
+          <t>Success. the Directory and its Content Deleted!</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>20:08:53</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E381" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\</t>
+        </is>
+      </c>
+      <c r="F381" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>20:08:54</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E382" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\..</t>
+        </is>
+      </c>
+      <c r="F382" s="3" t="inlineStr">
+        <is>
+          <t>Failed. Try Reaching the Root!</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>20:08:55</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E383" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\..</t>
+        </is>
+      </c>
+      <c r="F383" s="3" t="inlineStr">
+        <is>
+          <t>Failed. Try Reaching the Root!</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>20:09:13</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>DED</t>
+        </is>
+      </c>
+      <c r="E384" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\apple\</t>
+        </is>
+      </c>
+      <c r="F384" s="2" t="inlineStr">
+        <is>
+          <t>Success. the Directory Deleted!</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>20:12:42</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>mjavadtataro</t>
+        </is>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E385" t="inlineStr">
+        <is>
+          <t>pass: mjavadtataro</t>
+        </is>
+      </c>
+      <c r="F385" s="3" t="inlineStr">
+        <is>
+          <t>Failed Attempts= 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>20:12:43</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>mjavadtataro</t>
+        </is>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pass: </t>
+        </is>
+      </c>
+      <c r="F386" s="3" t="inlineStr">
+        <is>
+          <t>Failed Attempts= 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>20:12:46</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E387" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F387" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>20:13:52</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E388" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F388" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>20:13:57</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t>HELP</t>
+        </is>
+      </c>
+      <c r="E389" t="inlineStr">
+        <is>
+          <t>help ded</t>
+        </is>
+      </c>
+      <c r="F389" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>20:15:04</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>help ded</t>
+        </is>
+      </c>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E390" t="inlineStr">
+        <is>
+          <t>pass: help ded</t>
+        </is>
+      </c>
+      <c r="F390" s="3" t="inlineStr">
+        <is>
+          <t>Failed Attempts= 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>20:15:09</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D391" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E391" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F391" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>20:15:11</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D392" t="inlineStr">
+        <is>
+          <t>HELP</t>
+        </is>
+      </c>
+      <c r="E392" t="inlineStr">
+        <is>
+          <t>help ded</t>
+        </is>
+      </c>
+      <c r="F392" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>20:22:11</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D393" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E393" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F393" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>20:22:13</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D394" t="inlineStr">
+        <is>
+          <t>HELP</t>
+        </is>
+      </c>
+      <c r="E394" t="inlineStr">
+        <is>
+          <t>help ded</t>
+        </is>
+      </c>
+      <c r="F394" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>20:22:20</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D395" t="inlineStr">
+        <is>
+          <t>HELP</t>
+        </is>
+      </c>
+      <c r="E395" t="inlineStr">
+        <is>
+          <t>help add</t>
+        </is>
+      </c>
+      <c r="F395" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>20:22:23</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t>HELP</t>
+        </is>
+      </c>
+      <c r="E396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">help </t>
+        </is>
+      </c>
+      <c r="F396" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>20:22:26</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>HELP</t>
+        </is>
+      </c>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>help</t>
+        </is>
+      </c>
+      <c r="F397" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>20:22:31</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>HELP</t>
+        </is>
+      </c>
+      <c r="E398" t="inlineStr">
+        <is>
+          <t>help ded</t>
+        </is>
+      </c>
+      <c r="F398" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>20:22:56</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E399" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F399" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>20:24:19</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D400" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E400" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F400" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>20:24:21</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D401" t="inlineStr">
+        <is>
+          <t>HELP</t>
+        </is>
+      </c>
+      <c r="E401" t="inlineStr">
+        <is>
+          <t>help ded</t>
+        </is>
+      </c>
+      <c r="F401" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>20:24:40</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D402" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E402" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F402" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>20:24:42</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D403" t="inlineStr">
+        <is>
+          <t>HELP</t>
+        </is>
+      </c>
+      <c r="E403" t="inlineStr">
+        <is>
+          <t>help ded</t>
+        </is>
+      </c>
+      <c r="F403" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>20:25:25</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D404" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E404" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F404" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>20:25:28</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D405" t="inlineStr">
+        <is>
+          <t>HELP</t>
+        </is>
+      </c>
+      <c r="E405" t="inlineStr">
+        <is>
+          <t>help ded</t>
+        </is>
+      </c>
+      <c r="F405" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>20:25:55</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D406" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E406" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F406" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>20:25:57</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D407" t="inlineStr">
+        <is>
+          <t>HELP</t>
+        </is>
+      </c>
+      <c r="E407" t="inlineStr">
+        <is>
+          <t>help ded</t>
+        </is>
+      </c>
+      <c r="F407" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>20:27:01</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D408" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E408" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F408" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>20:27:03</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D409" t="inlineStr">
+        <is>
+          <t>HELP</t>
+        </is>
+      </c>
+      <c r="E409" t="inlineStr">
+        <is>
+          <t>help ded</t>
+        </is>
+      </c>
+      <c r="F409" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>20:29:04</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D410" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E410" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F410" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>20:29:06</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D411" t="inlineStr">
+        <is>
+          <t>DED</t>
+        </is>
+      </c>
+      <c r="F411" s="3" t="inlineStr">
+        <is>
+          <t>Failed. Empty Input!</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>20:32:41</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D412" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E412" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F412" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>20:32:43</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D413" t="inlineStr">
+        <is>
+          <t>HOME</t>
+        </is>
+      </c>
+      <c r="E413" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F413" s="2" t="inlineStr">
+        <is>
+          <t>Directory Changed Successfully</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>20:34:34</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D414" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E414" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F414" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>20:34:37</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D415" t="inlineStr">
+        <is>
+          <t>SUBD</t>
+        </is>
+      </c>
+      <c r="F415" s="2" t="inlineStr">
+        <is>
+          <t>Success. Sub-Directories and Files Showed-Up!</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>20:34:43</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D416" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E416" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F416" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>20:34:45</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D417" t="inlineStr">
+        <is>
+          <t>SUBD</t>
+        </is>
+      </c>
+      <c r="F417" s="2" t="inlineStr">
+        <is>
+          <t>Success. Sub-Directories and Files Showed-Up!</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>20:34:52</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D418" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E418" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\jj\</t>
+        </is>
+      </c>
+      <c r="F418" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>20:34:54</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D419" t="inlineStr">
+        <is>
+          <t>SUBD</t>
+        </is>
+      </c>
+      <c r="F419" s="2" t="inlineStr">
+        <is>
+          <t>Success. Sub-Directories and Files Showed-Up!</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>20:35:02</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D420" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E420" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\jj\jj3\</t>
+        </is>
+      </c>
+      <c r="F420" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>20:36:36</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D421" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E421" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F421" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>20:36:39</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D422" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E422" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F422" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>20:36:42</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D423" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E423" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\jj\</t>
+        </is>
+      </c>
+      <c r="F423" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>20:36:44</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D424" t="inlineStr">
+        <is>
+          <t>SUBD</t>
+        </is>
+      </c>
+      <c r="F424" s="2" t="inlineStr">
+        <is>
+          <t>Success. Sub-Directories and Files Showed-Up!</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>20:36:50</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D425" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E425" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\jj\jj3\</t>
+        </is>
+      </c>
+      <c r="F425" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>2021/05/07</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>20:36:52</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D426" t="inlineStr">
+        <is>
+          <t>SUBD</t>
+        </is>
+      </c>
+      <c r="E426" t="inlineStr"/>
+      <c r="F426" s="2" t="inlineStr">
+        <is>
+          <t>Success. Sub-Directories and Files Showed-Up!</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
addint two commands: CPD & MVD
</commit_message>
<xml_diff>
--- a/root/administrator/logs_file.xlsx
+++ b/root/administrator/logs_file.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F426"/>
+  <dimension ref="A1:F464"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13990,10 +13990,1210 @@
           <t>SUBD</t>
         </is>
       </c>
-      <c r="E426" t="inlineStr"/>
       <c r="F426" s="2" t="inlineStr">
         <is>
           <t>Success. Sub-Directories and Files Showed-Up!</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>17:30:53</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D427" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E427" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F427" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>17:31:57</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D428" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E428" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F428" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>17:33:21</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D429" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E429" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F429" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>17:33:25</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D430" t="inlineStr">
+        <is>
+          <t>SUBD</t>
+        </is>
+      </c>
+      <c r="F430" s="2" t="inlineStr">
+        <is>
+          <t>Success. Sub-Directories and Files Showed-Up!</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>17:33:29</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D431" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E431" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F431" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>17:33:32</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D432" t="inlineStr">
+        <is>
+          <t>SUBD</t>
+        </is>
+      </c>
+      <c r="F432" s="2" t="inlineStr">
+        <is>
+          <t>Success. Sub-Directories and Files Showed-Up!</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>17:33:38</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D433" t="inlineStr">
+        <is>
+          <t>CHD</t>
+        </is>
+      </c>
+      <c r="E433" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\jjj\</t>
+        </is>
+      </c>
+      <c r="F433" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Changed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>17:33:41</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D434" t="inlineStr">
+        <is>
+          <t>SUBD</t>
+        </is>
+      </c>
+      <c r="F434" s="2" t="inlineStr">
+        <is>
+          <t>Success. Sub-Directories and Files Showed-Up!</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>17:34:45</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D435" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E435" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F435" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>17:35:21</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D436" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E436" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F436" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>17:38:54</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E437" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F437" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>17:39:08</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E438" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F438" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>17:39:11</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D439" t="inlineStr">
+        <is>
+          <t>CPD</t>
+        </is>
+      </c>
+      <c r="E439" t="inlineStr">
+        <is>
+          <t>['ad']</t>
+        </is>
+      </c>
+      <c r="F439" s="3" t="inlineStr">
+        <is>
+          <t>Failed. Invalid Parameters!</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>17:39:17</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D440" t="inlineStr">
+        <is>
+          <t>HELP</t>
+        </is>
+      </c>
+      <c r="E440" t="inlineStr">
+        <is>
+          <t>help cpd</t>
+        </is>
+      </c>
+      <c r="F440" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>17:40:44</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D441" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E441" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F441" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>17:40:47</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D442" t="inlineStr">
+        <is>
+          <t>CPD</t>
+        </is>
+      </c>
+      <c r="E442" t="inlineStr">
+        <is>
+          <t>['s']</t>
+        </is>
+      </c>
+      <c r="F442" s="3" t="inlineStr">
+        <is>
+          <t>Failed. Invalid Parameters!</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>17:41:24</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D443" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E443" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F443" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>17:42:10</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D444" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E444" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F444" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>17:42:40</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D445" t="inlineStr">
+        <is>
+          <t>CPD</t>
+        </is>
+      </c>
+      <c r="E445" t="inlineStr">
+        <is>
+          <t>['mjavadtatari\\home\\jj', 'cpd', 'mjavadtatari\\home\\jjj']</t>
+        </is>
+      </c>
+      <c r="F445" s="3" t="inlineStr">
+        <is>
+          <t>Failed. Invalid Parameters!</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>17:42:50</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D446" t="inlineStr">
+        <is>
+          <t>CPD</t>
+        </is>
+      </c>
+      <c r="E446" t="inlineStr">
+        <is>
+          <t>['mjavadtatari\\home\\jj', 'cpd', 'mjavadtatari\\home\\jjj']</t>
+        </is>
+      </c>
+      <c r="F446" s="3" t="inlineStr">
+        <is>
+          <t>Failed. Invalid Parameters!</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>17:45:19</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D447" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E447" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F447" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>17:45:26</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D448" t="inlineStr">
+        <is>
+          <t>CPD</t>
+        </is>
+      </c>
+      <c r="E448" t="inlineStr">
+        <is>
+          <t>root\mjasdtoroot\sadas</t>
+        </is>
+      </c>
+      <c r="F448" s="3" t="inlineStr">
+        <is>
+          <t>Failed. Directory Not Found!</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>17:45:43</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D449" t="inlineStr">
+        <is>
+          <t>CPD</t>
+        </is>
+      </c>
+      <c r="E449" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\hometoroot\mjavadtatari\home</t>
+        </is>
+      </c>
+      <c r="F449" s="3" t="inlineStr">
+        <is>
+          <t>Failed. Directory Already Exist!</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>17:48:22</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D450" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E450" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F450" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>17:48:50</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D451" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E451" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F451" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>17:48:53</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D452" t="inlineStr">
+        <is>
+          <t>CPD</t>
+        </is>
+      </c>
+      <c r="E452" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fasf, asfas, fas, dasd, </t>
+        </is>
+      </c>
+      <c r="F452" s="3" t="inlineStr">
+        <is>
+          <t>Failed. Invalid Parameters!</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>17:49:51</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D453" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E453" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F453" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>17:49:57</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D454" t="inlineStr">
+        <is>
+          <t>CPD</t>
+        </is>
+      </c>
+      <c r="E454" t="inlineStr">
+        <is>
+          <t xml:space="preserve">sadasd\sdsd\sd, sdasdac, c\dcdc, df, </t>
+        </is>
+      </c>
+      <c r="F454" s="3" t="inlineStr">
+        <is>
+          <t>Failed. Invalid Parameters!</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>17:52:02</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D455" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E455" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F455" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>17:52:27</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D456" t="inlineStr">
+        <is>
+          <t>CPD</t>
+        </is>
+      </c>
+      <c r="E456" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\jj --&gt; root\mjavadtatari\home\hello</t>
+        </is>
+      </c>
+      <c r="F456" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Copied!</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>17:56:41</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D457" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E457" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F457" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>17:56:46</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D458" t="inlineStr">
+        <is>
+          <t>MVD</t>
+        </is>
+      </c>
+      <c r="E458" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mjavadtatari, </t>
+        </is>
+      </c>
+      <c r="F458" s="3" t="inlineStr">
+        <is>
+          <t>Failed. Invalid Parameters!</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>17:57:53</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D459" t="inlineStr">
+        <is>
+          <t>MVD</t>
+        </is>
+      </c>
+      <c r="E459" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\one\three --&gt; root\mjavadtatari\home\two\three</t>
+        </is>
+      </c>
+      <c r="F459" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Moved!</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>17:58:53</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D460" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E460" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F460" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>17:59:24</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D461" t="inlineStr">
+        <is>
+          <t>MVD</t>
+        </is>
+      </c>
+      <c r="E461" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\one --&gt; root\mjavadtatari\home\two\three</t>
+        </is>
+      </c>
+      <c r="F461" s="2" t="inlineStr">
+        <is>
+          <t>Success. Directory Moved!</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>18:00:55</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>mjavadtatarti</t>
+        </is>
+      </c>
+      <c r="D462" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E462" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatarti</t>
+        </is>
+      </c>
+      <c r="F462" s="3" t="inlineStr">
+        <is>
+          <t>Failed Attempts= 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>18:00:58</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D463" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E463" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F463" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>2021/05/09</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>18:01:06</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D464" t="inlineStr">
+        <is>
+          <t>MVD</t>
+        </is>
+      </c>
+      <c r="E464" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\one --&gt; root\mjavadtatari\home\two\three</t>
+        </is>
+      </c>
+      <c r="F464" s="3" t="inlineStr">
+        <is>
+          <t>Failed. Directory Already Exist!</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adding CPF & MVF commands.
</commit_message>
<xml_diff>
--- a/root/administrator/logs_file.xlsx
+++ b/root/administrator/logs_file.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F189"/>
+  <dimension ref="A1:F224"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6442,6 +6442,1126 @@
         </is>
       </c>
     </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>01:54:41</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F190" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>01:54:46</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\jj.txt</t>
+        </is>
+      </c>
+      <c r="F191" s="3" t="inlineStr">
+        <is>
+          <t>Failed. File Not Found!</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>01:54:54</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>HOME</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F192" s="2" t="inlineStr">
+        <is>
+          <t>Directory Changed Successfully</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>01:54:57</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\jj.txt</t>
+        </is>
+      </c>
+      <c r="F193" s="2" t="inlineStr">
+        <is>
+          <t>Success. File Removed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>01:55:00</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\jj.txt</t>
+        </is>
+      </c>
+      <c r="F194" s="3" t="inlineStr">
+        <is>
+          <t>Failed. File Not Found!</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>01:56:09</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F195" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>01:56:29</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>root\U1030\home\d.txt</t>
+        </is>
+      </c>
+      <c r="F196" s="2" t="inlineStr">
+        <is>
+          <t>Success. File Removed!</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>01:58:01</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F197" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>01:58:11</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>DEF</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\U1030\home\asd.txt</t>
+        </is>
+      </c>
+      <c r="F198" s="3" t="inlineStr">
+        <is>
+          <t>Failed. File Not Found!</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>02:00:20</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F199" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>02:00:29</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>MKD</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>U1030\home\hell\</t>
+        </is>
+      </c>
+      <c r="F200" s="3" t="inlineStr">
+        <is>
+          <t>Fail. Not Valid!</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>02:00:54</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>DED</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\U1030\home\</t>
+        </is>
+      </c>
+      <c r="F201" s="3" t="inlineStr">
+        <is>
+          <t>Failed. Directory Does Not Exists!</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>02:02:53</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>mjavadtatar</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatar</t>
+        </is>
+      </c>
+      <c r="F202" s="3" t="inlineStr">
+        <is>
+          <t>Failed Attempts= 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>02:02:55</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F203" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>02:03:03</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>HELP</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>help cpd</t>
+        </is>
+      </c>
+      <c r="F204" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>02:09:51</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F205" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>02:10:06</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>CPF</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t xml:space="preserve">, </t>
+        </is>
+      </c>
+      <c r="F206" s="3" t="inlineStr">
+        <is>
+          <t>Failed. Invalid Parameters!</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>02:11:34</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F207" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>02:11:37</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>HOME</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F208" s="2" t="inlineStr">
+        <is>
+          <t>Directory Changed Successfully</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>02:11:49</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>CPF</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\1.txt --&gt; root\mjavadtatari\home\2.txt</t>
+        </is>
+      </c>
+      <c r="F209" s="2" t="inlineStr">
+        <is>
+          <t>Success. File Copied!</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>02:12:01</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>CPF</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\1.txt --&gt; root\mjavadtatari\home\2.txt</t>
+        </is>
+      </c>
+      <c r="F210" s="2" t="inlineStr">
+        <is>
+          <t>Success. File Copied!</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>02:13:31</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F211" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>02:13:51</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>CPF</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\1.txt --&gt; root\mjavadtatari\home\3.txt</t>
+        </is>
+      </c>
+      <c r="F212" s="2" t="inlineStr">
+        <is>
+          <t>Success. File Copied!</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>02:13:54</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>CPF</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\1.txt --&gt; root\mjavadtatari\home\3.txt</t>
+        </is>
+      </c>
+      <c r="F213" s="3" t="inlineStr">
+        <is>
+          <t>Failed. File Already Exists!</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>02:15:29</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F214" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>02:15:46</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>CPF</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\12.txt --&gt; root\mjavadtatari\home\5.txt</t>
+        </is>
+      </c>
+      <c r="F215" s="3" t="inlineStr">
+        <is>
+          <t>Failed. File Not Found!</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>02:15:51</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>CPF</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\1.txt --&gt; root\mjavadtatari\home\5.txt</t>
+        </is>
+      </c>
+      <c r="F216" s="2" t="inlineStr">
+        <is>
+          <t>Success. File Copied!</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>02:15:53</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>CPF</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\1.txt --&gt; root\mjavadtatari\home\5.txt</t>
+        </is>
+      </c>
+      <c r="F217" s="3" t="inlineStr">
+        <is>
+          <t>Failed. File Already Exists!</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>02:18:20</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>pass: mjavadtatari</t>
+        </is>
+      </c>
+      <c r="F218" s="2" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>02:18:22</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>HOME</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\</t>
+        </is>
+      </c>
+      <c r="F219" s="2" t="inlineStr">
+        <is>
+          <t>Directory Changed Successfully</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>02:18:23</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>SHOW</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+      <c r="F220" s="2" t="inlineStr">
+        <is>
+          <t>Success. Sub-Directories and Files Showed-Up!</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>02:18:45</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>MVF</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\3.txt --&gt; root\mjavadtatari\home\well\3.txt</t>
+        </is>
+      </c>
+      <c r="F221" s="2" t="inlineStr">
+        <is>
+          <t>Success. File Moved!</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>02:19:00</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>SHOW</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>show</t>
+        </is>
+      </c>
+      <c r="F222" s="2" t="inlineStr">
+        <is>
+          <t>Success. Sub-Directories and Files Showed-Up!</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>02:19:02</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>MVF</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\3.txt --&gt; root\mjavadtatari\home\well\3.txt</t>
+        </is>
+      </c>
+      <c r="F223" s="3" t="inlineStr">
+        <is>
+          <t>Failed. File Not Found!</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>2021/05/16</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>02:19:13</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>mjavadtatari</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>MVF</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>root\mjavadtatari\home\2.txt --&gt; root\mjavadtatari\home\well\3.txt</t>
+        </is>
+      </c>
+      <c r="F224" s="3" t="inlineStr">
+        <is>
+          <t>Failed. File Already Exists!</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>